<commit_message>
Table 2 and 3 .xlsx files corrected for domain analysis.
</commit_message>
<xml_diff>
--- a/table2.xlsx
+++ b/table2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>Effect</t>
   </si>
@@ -320,6 +320,72 @@
   </si>
   <si>
     <t>exp_estimate</t>
+  </si>
+  <si>
+    <t>effect</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>25-29</t>
+  </si>
+  <si>
+    <t>30-34</t>
+  </si>
+  <si>
+    <t>35-39</t>
+  </si>
+  <si>
+    <t>40-44</t>
+  </si>
+  <si>
+    <t>45-49</t>
+  </si>
+  <si>
+    <t>50-54</t>
+  </si>
+  <si>
+    <t>55-59</t>
+  </si>
+  <si>
+    <t>60-64</t>
+  </si>
+  <si>
+    <t>65-69</t>
+  </si>
+  <si>
+    <t>70-74</t>
+  </si>
+  <si>
+    <t>75-79</t>
+  </si>
+  <si>
+    <t>80+</t>
+  </si>
+  <si>
+    <t>birth_control</t>
+  </si>
+  <si>
+    <t>N/A (Male)</t>
+  </si>
+  <si>
+    <t>cotinine_cat</t>
+  </si>
+  <si>
+    <t>3+ ng/mL</t>
+  </si>
+  <si>
+    <t>&lt;3 ng/mL</t>
+  </si>
+  <si>
+    <t>poor_sleep</t>
+  </si>
+  <si>
+    <t>short_sleep</t>
+  </si>
+  <si>
+    <t>sleep_med</t>
   </si>
 </sst>
 </file>
@@ -396,7 +462,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
@@ -405,7 +471,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -428,13 +494,13 @@
         <v>69</v>
       </c>
       <c r="C2">
-        <v>-1.5800207433195592</v>
+        <v>-1.5800207433195559</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
       </c>
       <c r="E2">
-        <v>.20597082564191388</v>
+        <v>.20597082564191455</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -445,13 +511,13 @@
         <v>70</v>
       </c>
       <c r="C3">
-        <v>-2.0219182374204845</v>
+        <v>-2.021918237420485</v>
       </c>
       <c r="D3" t="s">
         <v>68</v>
       </c>
       <c r="E3">
-        <v>.1324012443088248</v>
+        <v>.13240124430882474</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -462,13 +528,13 @@
         <v>71</v>
       </c>
       <c r="C4">
-        <v>-1.640805194535589</v>
+        <v>-1.640805194535592</v>
       </c>
       <c r="D4" t="s">
         <v>68</v>
       </c>
       <c r="E4">
-        <v>.19382391348629144</v>
+        <v>.19382391348629088</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -479,13 +545,13 @@
         <v>72</v>
       </c>
       <c r="C5">
-        <v>-1.5904691332565257</v>
+        <v>-1.590469133256529</v>
       </c>
       <c r="D5" t="s">
         <v>68</v>
       </c>
       <c r="E5">
-        <v>.2038299658849701</v>
+        <v>.20382996588496943</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -496,13 +562,13 @@
         <v>73</v>
       </c>
       <c r="C6">
-        <v>-1.743430984554211</v>
+        <v>-1.7434309845542093</v>
       </c>
       <c r="D6" t="s">
         <v>68</v>
       </c>
       <c r="E6">
-        <v>.17491922473584842</v>
+        <v>.17491922473584873</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -513,13 +579,13 @@
         <v>74</v>
       </c>
       <c r="C7">
-        <v>-1.6409825400950218</v>
+        <v>-1.6409825400950255</v>
       </c>
       <c r="D7" t="s">
         <v>68</v>
       </c>
       <c r="E7">
-        <v>.19378954272376392</v>
+        <v>.1937895427237632</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,13 +596,13 @@
         <v>75</v>
       </c>
       <c r="C8">
-        <v>-1.6423768566307722</v>
+        <v>-1.6423768566307746</v>
       </c>
       <c r="D8" t="s">
         <v>68</v>
       </c>
       <c r="E8">
-        <v>.1935195270472952</v>
+        <v>.1935195270472947</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -547,13 +613,13 @@
         <v>76</v>
       </c>
       <c r="C9">
-        <v>-1.833573879795681</v>
+        <v>-1.8335738797956798</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9">
-        <v>.15984129219753143</v>
+        <v>.15984129219753163</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,13 +630,13 @@
         <v>77</v>
       </c>
       <c r="C10">
-        <v>-1.6912554073416448</v>
+        <v>-1.6912554073416481</v>
       </c>
       <c r="D10" t="s">
         <v>68</v>
       </c>
       <c r="E10">
-        <v>.1842880221728388</v>
+        <v>.18428802217283818</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -581,13 +647,13 @@
         <v>78</v>
       </c>
       <c r="C11">
-        <v>-1.4525587389982013</v>
+        <v>-1.4525587389981984</v>
       </c>
       <c r="D11" t="s">
         <v>68</v>
       </c>
       <c r="E11">
-        <v>.2339708511781892</v>
+        <v>.2339708511781899</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -598,13 +664,13 @@
         <v>79</v>
       </c>
       <c r="C12">
-        <v>-1.8989002235008285</v>
+        <v>-1.8989002235008299</v>
       </c>
       <c r="D12" t="s">
         <v>68</v>
       </c>
       <c r="E12">
-        <v>.1497332017604846</v>
+        <v>.1497332017604844</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -615,13 +681,13 @@
         <v>80</v>
       </c>
       <c r="C13">
-        <v>-1.6233057754875664</v>
+        <v>-1.6233057754875642</v>
       </c>
       <c r="D13" t="s">
         <v>68</v>
       </c>
       <c r="E13">
-        <v>.19724557055808828</v>
+        <v>.1972455705580887</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -632,13 +698,13 @@
         <v>81</v>
       </c>
       <c r="C14">
-        <v>-1.9070463703536646</v>
+        <v>-1.9070463703536606</v>
       </c>
       <c r="D14" t="s">
         <v>68</v>
       </c>
       <c r="E14">
-        <v>.14851840777308084</v>
+        <v>.14851840777308142</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,13 +715,13 @@
         <v>82</v>
       </c>
       <c r="C15">
-        <v>-1.6180827610346444</v>
+        <v>-1.618082761034647</v>
       </c>
       <c r="D15" t="s">
         <v>68</v>
       </c>
       <c r="E15">
-        <v>.19827848213178606</v>
+        <v>.19827848213178556</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -666,13 +732,13 @@
         <v>83</v>
       </c>
       <c r="C16">
-        <v>-1.522607912578059</v>
+        <v>-1.5226079125780527</v>
       </c>
       <c r="D16" t="s">
         <v>68</v>
       </c>
       <c r="E16">
-        <v>.21814224857765444</v>
+        <v>.2181422485776558</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -683,13 +749,13 @@
         <v>84</v>
       </c>
       <c r="C17">
-        <v>-1.779968807284094</v>
+        <v>-1.779968807284091</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
       </c>
       <c r="E17">
-        <v>.16864340763245622</v>
+        <v>.16864340763245675</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -717,13 +783,13 @@
         <v>86</v>
       </c>
       <c r="C19">
-        <v>-2.1932529746488303</v>
+        <v>-2.1932529746488307</v>
       </c>
       <c r="D19" t="s">
         <v>68</v>
       </c>
       <c r="E19">
-        <v>.11155327777253495</v>
+        <v>.1115532777725349</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -731,16 +797,16 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="C20">
-        <v>-2.152619564473262</v>
+        <v>-2.1526195644732598</v>
       </c>
       <c r="D20" t="s">
         <v>68</v>
       </c>
       <c r="E20">
-        <v>.11617941932736178</v>
+        <v>.11617941932736205</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -748,16 +814,16 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C21">
-        <v>-1.98029409416184</v>
+        <v>-1.9802940941618412</v>
       </c>
       <c r="D21" t="s">
         <v>68</v>
       </c>
       <c r="E21">
-        <v>.1380286379245838</v>
+        <v>.13802863792458364</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -765,16 +831,16 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C22">
-        <v>-1.9060596356826447</v>
+        <v>-1.906059635682643</v>
       </c>
       <c r="D22" t="s">
         <v>68</v>
       </c>
       <c r="E22">
-        <v>.14866502836122775</v>
+        <v>.148665028361228</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -782,16 +848,16 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="C23">
-        <v>-1.8967331615072405</v>
+        <v>-1.8967331615072418</v>
       </c>
       <c r="D23" t="s">
         <v>68</v>
       </c>
       <c r="E23">
-        <v>.15005803473066776</v>
+        <v>.15005803473066753</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -799,16 +865,16 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C24">
-        <v>-1.7590877876552025</v>
+        <v>-1.7590877876552038</v>
       </c>
       <c r="D24" t="s">
         <v>68</v>
       </c>
       <c r="E24">
-        <v>.17220187687542327</v>
+        <v>.17220187687542304</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,16 +882,16 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C25">
-        <v>-1.6862771204385463</v>
+        <v>-1.6862771204385452</v>
       </c>
       <c r="D25" t="s">
         <v>68</v>
       </c>
       <c r="E25">
-        <v>.18520774825067401</v>
+        <v>.18520774825067424</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -833,16 +899,16 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="C26">
-        <v>-1.7077692497635393</v>
+        <v>-1.7077692497635355</v>
       </c>
       <c r="D26" t="s">
         <v>68</v>
       </c>
       <c r="E26">
-        <v>.18126970937797615</v>
+        <v>.18126970937797685</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -850,16 +916,16 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="C27">
-        <v>-1.658025486896768</v>
+        <v>-1.6580254868967692</v>
       </c>
       <c r="D27" t="s">
         <v>68</v>
       </c>
       <c r="E27">
-        <v>.1905147829008466</v>
+        <v>.19051478290084642</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -867,16 +933,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="C28">
-        <v>-1.504766767943969</v>
+        <v>-1.5047667679439711</v>
       </c>
       <c r="D28" t="s">
         <v>68</v>
       </c>
       <c r="E28">
-        <v>.22206908142089243</v>
+        <v>.22206908142089196</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -884,16 +950,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="C29">
-        <v>-1.5553399773960823</v>
+        <v>-1.555339977396083</v>
       </c>
       <c r="D29" t="s">
         <v>68</v>
       </c>
       <c r="E29">
-        <v>.2111175952283209</v>
+        <v>.21111759522832077</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,16 +967,16 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="C30">
-        <v>-1.4883956629187047</v>
+        <v>-1.488395662918704</v>
       </c>
       <c r="D30" t="s">
         <v>68</v>
       </c>
       <c r="E30">
-        <v>.2257345194460558</v>
+        <v>.22573451944605594</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,16 +984,16 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="C31">
-        <v>-1.5454726123548628</v>
+        <v>-1.5454726123548632</v>
       </c>
       <c r="D31" t="s">
         <v>68</v>
       </c>
       <c r="E31">
-        <v>.2132110812163136</v>
+        <v>.2132110812163135</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -935,75 +1001,75 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="C32">
-        <v>-1.5433303973343977</v>
+        <v>-1.5433303973344006</v>
       </c>
       <c r="D32" t="s">
         <v>68</v>
       </c>
       <c r="E32">
-        <v>.21366831476845946</v>
+        <v>.21366831476845885</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C33">
-        <v>-1.7062138838410728</v>
+        <v>-1.7062138838410743</v>
       </c>
       <c r="D33" t="s">
         <v>68</v>
       </c>
       <c r="E33">
-        <v>.18155186948093988</v>
+        <v>.1815518694809396</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C34">
-        <v>-1.9070463703536646</v>
+        <v>-1.9070463703536606</v>
       </c>
       <c r="D34" t="s">
         <v>68</v>
       </c>
       <c r="E34">
-        <v>.14851840777308084</v>
+        <v>.14851840777308142</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C35">
-        <v>-1.6576575272455145</v>
+        <v>-1.65765752724551</v>
       </c>
       <c r="D35" t="s">
         <v>68</v>
       </c>
       <c r="E35">
-        <v>.1905848975528118</v>
+        <v>.19058489755281266</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C36">
         <v>-1.2064941997322796</v>
@@ -1017,10 +1083,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="C37">
         <v>-1.7263405832988739</v>
@@ -1034,19 +1100,19 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C38">
-        <v>-1.7757671779129203</v>
+        <v>-1.7757671779129143</v>
       </c>
       <c r="D38" t="s">
         <v>68</v>
       </c>
       <c r="E38">
-        <v>.16935347540341122</v>
+        <v>.16935347540341225</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1054,16 +1120,16 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="C39">
-        <v>-1.6831835347816093</v>
+        <v>-1.6831835347816113</v>
       </c>
       <c r="D39" t="s">
         <v>68</v>
       </c>
       <c r="E39">
-        <v>.18578159144309772</v>
+        <v>.18578159144309736</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,16 +1137,16 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="C40">
-        <v>-1.9070463703536646</v>
+        <v>-1.9070463703536606</v>
       </c>
       <c r="D40" t="s">
         <v>68</v>
       </c>
       <c r="E40">
-        <v>.14851840777308084</v>
+        <v>.14851840777308142</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1088,16 +1154,16 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C41">
-        <v>-1.6352298292339107</v>
+        <v>-1.6352298292339091</v>
       </c>
       <c r="D41" t="s">
         <v>68</v>
       </c>
       <c r="E41">
-        <v>.19490757069347936</v>
+        <v>.19490757069347966</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1105,16 +1171,16 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="C42">
-        <v>-1.2097903091532884</v>
+        <v>-1.2097903091532887</v>
       </c>
       <c r="D42" t="s">
         <v>68</v>
       </c>
       <c r="E42">
-        <v>.298259815226261</v>
+        <v>.29825981522626094</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1122,16 +1188,16 @@
         <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C43">
-        <v>-2.11743594984831</v>
+        <v>-2.1174359498482964</v>
       </c>
       <c r="D43" t="s">
         <v>68</v>
       </c>
       <c r="E43">
-        <v>.12033979052935298</v>
+        <v>.12033979052935463</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,75 +1205,75 @@
         <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C44">
-        <v>-1.0773206628727308</v>
+        <v>-1.077320662872732</v>
       </c>
       <c r="D44" t="s">
         <v>68</v>
       </c>
       <c r="E44">
-        <v>.3405066365866803</v>
+        <v>.3405066365866798</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C45">
-        <v>-1.807395504655218</v>
+        <v>-1.807395504655211</v>
       </c>
       <c r="D45" t="s">
         <v>68</v>
       </c>
       <c r="E45">
-        <v>.16408092878777195</v>
+        <v>.16408092878777306</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C46">
-        <v>-1.7172157021781307</v>
+        <v>-1.7172157021781318</v>
       </c>
       <c r="D46" t="s">
         <v>68</v>
       </c>
       <c r="E46">
-        <v>.1795654161302604</v>
+        <v>.17956541613026022</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C47">
-        <v>-1.7897044289555046</v>
+        <v>-1.7897044289554993</v>
       </c>
       <c r="D47" t="s">
         <v>68</v>
       </c>
       <c r="E47">
-        <v>.16700952555250428</v>
+        <v>.16700952555250514</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C48">
         <v>-1.5880890122241196</v>
@@ -1221,53 +1287,53 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C49">
-        <v>-1.3786286147946523</v>
+        <v>-1.3786286147946516</v>
       </c>
       <c r="D49" t="s">
         <v>68</v>
       </c>
       <c r="E49">
-        <v>.2519238008451491</v>
+        <v>.25192380084514926</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C50">
-        <v>-1.7856349907934517</v>
+        <v>-1.7856349907934523</v>
       </c>
       <c r="D50" t="s">
         <v>68</v>
       </c>
       <c r="E50">
-        <v>.16769054523312726</v>
+        <v>.16769054523312715</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="C51">
-        <v>-1.6597536110576852</v>
+        <v>-1.6597536110576874</v>
       </c>
       <c r="D51" t="s">
         <v>68</v>
       </c>
       <c r="E51">
-        <v>.1901858340156267</v>
+        <v>.19018583401562628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>